<commit_message>
Final Results Added to json
</commit_message>
<xml_diff>
--- a/isp_status.xlsx
+++ b/isp_status.xlsx
@@ -433,22 +433,22 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B2" t="str">
-        <v>Agrabad</v>
+        <v>Nawabpur</v>
       </c>
       <c r="C2" t="str">
-        <v>192.168.129.1</v>
+        <v>192.168.18.1</v>
       </c>
       <c r="D2" t="str">
-        <v>BDCOM</v>
+        <v>ALAP</v>
       </c>
       <c r="E2" t="str">
         <v>DOWN</v>
       </c>
       <c r="F2" t="str">
-        <v>ALAP</v>
+        <v>KS</v>
       </c>
       <c r="G2" t="str">
         <v>DOWN</v>
@@ -457,27 +457,27 @@
         <v>OK</v>
       </c>
       <c r="I2" t="str">
-        <v>legacy</v>
+        <v>sdwan</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B3" t="str">
-        <v>Barisal</v>
+        <v>Corporate</v>
       </c>
       <c r="C3" t="str">
-        <v>192.168.241.1</v>
+        <v>192.168.15.1</v>
       </c>
       <c r="D3" t="str">
-        <v>ALAP</v>
+        <v>BDCOM</v>
       </c>
       <c r="E3" t="str">
         <v>DOWN</v>
       </c>
       <c r="F3" t="str">
-        <v>BDCOM</v>
+        <v>ALAP</v>
       </c>
       <c r="G3" t="str">
         <v>DOWN</v>
@@ -491,22 +491,22 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B4" t="str">
-        <v>Khulna</v>
+        <v>New Elephant Road</v>
       </c>
       <c r="C4" t="str">
-        <v>192.168.225.1</v>
+        <v>192.168.16.1</v>
       </c>
       <c r="D4" t="str">
-        <v xml:space="preserve">BDCOM </v>
+        <v>ADN</v>
       </c>
       <c r="E4" t="str">
         <v>DOWN</v>
       </c>
       <c r="F4" t="str">
-        <v>ALAP</v>
+        <v>Alap</v>
       </c>
       <c r="G4" t="str">
         <v>DOWN</v>
@@ -520,16 +520,16 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B5" t="str">
-        <v>Moulvibazar, Dhaka</v>
+        <v>VIP Road</v>
       </c>
       <c r="C5" t="str">
-        <v>192.168.12.1</v>
+        <v>192.168.14.1</v>
       </c>
       <c r="D5" t="str">
-        <v>KS</v>
+        <v>BDCOM</v>
       </c>
       <c r="E5" t="str">
         <v>DOWN</v>
@@ -544,7 +544,7 @@
         <v>OK</v>
       </c>
       <c r="I5" t="str">
-        <v>legacy</v>
+        <v>sdwan</v>
       </c>
     </row>
     <row r="6">
@@ -578,16 +578,16 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B7" t="str">
-        <v>Bogra</v>
+        <v>Moulvibazar, Dhaka</v>
       </c>
       <c r="C7" t="str">
-        <v>192.168.162.1</v>
+        <v>192.168.12.1</v>
       </c>
       <c r="D7" t="str">
-        <v>BDCOM</v>
+        <v>KS</v>
       </c>
       <c r="E7" t="str">
         <v>DOWN</v>
@@ -607,13 +607,13 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B8" t="str">
-        <v>VIP Road</v>
+        <v>Agrabad</v>
       </c>
       <c r="C8" t="str">
-        <v>192.168.14.1</v>
+        <v>192.168.129.1</v>
       </c>
       <c r="D8" t="str">
         <v>BDCOM</v>
@@ -631,7 +631,7 @@
         <v>OK</v>
       </c>
       <c r="I8" t="str">
-        <v>sdwan</v>
+        <v>legacy</v>
       </c>
     </row>
     <row r="9">
@@ -694,22 +694,22 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="str">
-        <v>Khatungonj</v>
+        <v>Barisal</v>
       </c>
       <c r="C11" t="str">
-        <v>192.168.130.1</v>
+        <v>192.168.241.1</v>
       </c>
       <c r="D11" t="str">
-        <v>BDCOM</v>
+        <v>ALAP</v>
       </c>
       <c r="E11" t="str">
         <v>DOWN</v>
       </c>
       <c r="F11" t="str">
-        <v>ALAP</v>
+        <v>BDCOM</v>
       </c>
       <c r="G11" t="str">
         <v>DOWN</v>
@@ -718,21 +718,21 @@
         <v>OK</v>
       </c>
       <c r="I11" t="str">
-        <v>sdwan</v>
+        <v>legacy</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B12" t="str">
-        <v>Corporate</v>
+        <v>Khulna</v>
       </c>
       <c r="C12" t="str">
-        <v>192.168.15.1</v>
+        <v>192.168.225.1</v>
       </c>
       <c r="D12" t="str">
-        <v>BDCOM</v>
+        <v xml:space="preserve">BDCOM </v>
       </c>
       <c r="E12" t="str">
         <v>DOWN</v>
@@ -747,27 +747,27 @@
         <v>OK</v>
       </c>
       <c r="I12" t="str">
-        <v>legacy</v>
+        <v>sdwan</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B13" t="str">
-        <v>New Elephant Road</v>
+        <v>Satkhira</v>
       </c>
       <c r="C13" t="str">
-        <v>192.168.16.1</v>
+        <v>192.168.226.1</v>
       </c>
       <c r="D13" t="str">
-        <v>ADN</v>
+        <v>ALAP</v>
       </c>
       <c r="E13" t="str">
         <v>DOWN</v>
       </c>
       <c r="F13" t="str">
-        <v>Alap</v>
+        <v>AMBER-IT</v>
       </c>
       <c r="G13" t="str">
         <v>DOWN</v>
@@ -776,18 +776,18 @@
         <v>OK</v>
       </c>
       <c r="I13" t="str">
-        <v>sdwan</v>
+        <v>legacy</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B14" t="str">
-        <v>Benapole</v>
+        <v>Khatungonj</v>
       </c>
       <c r="C14" t="str">
-        <v>192.168.227.1</v>
+        <v>192.168.130.1</v>
       </c>
       <c r="D14" t="str">
         <v>BDCOM</v>
@@ -810,22 +810,22 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B15" t="str">
-        <v>Satkhira</v>
+        <v>Bogra</v>
       </c>
       <c r="C15" t="str">
-        <v>192.168.226.1</v>
+        <v>192.168.162.1</v>
       </c>
       <c r="D15" t="str">
-        <v>ALAP</v>
+        <v>BDCOM</v>
       </c>
       <c r="E15" t="str">
         <v>DOWN</v>
       </c>
       <c r="F15" t="str">
-        <v>AMBER-IT</v>
+        <v>ALAP</v>
       </c>
       <c r="G15" t="str">
         <v>DOWN</v>
@@ -839,22 +839,22 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B16" t="str">
-        <v>Nawabpur</v>
+        <v>Benapole</v>
       </c>
       <c r="C16" t="str">
-        <v>192.168.18.1</v>
+        <v>192.168.227.1</v>
       </c>
       <c r="D16" t="str">
-        <v>ALAP</v>
+        <v>BDCOM</v>
       </c>
       <c r="E16" t="str">
         <v>DOWN</v>
       </c>
       <c r="F16" t="str">
-        <v>KS</v>
+        <v>ALAP</v>
       </c>
       <c r="G16" t="str">
         <v>DOWN</v>
@@ -868,22 +868,22 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B17" t="str">
-        <v>Uttara</v>
+        <v>North South Road</v>
       </c>
       <c r="C17" t="str">
-        <v>192.168.17.1</v>
+        <v>192.168.13.1</v>
       </c>
       <c r="D17" t="str">
-        <v>Bdcom</v>
+        <v>ADN</v>
       </c>
       <c r="E17" t="str">
         <v>DOWN</v>
       </c>
       <c r="F17" t="str">
-        <v>Alap</v>
+        <v>ALAP</v>
       </c>
       <c r="G17" t="str">
         <v>DOWN</v>
@@ -892,7 +892,7 @@
         <v>OK</v>
       </c>
       <c r="I17" t="str">
-        <v>sdwan</v>
+        <v>legacy</v>
       </c>
     </row>
     <row r="18">
@@ -926,13 +926,13 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B19" t="str">
-        <v>Zindabazar</v>
+        <v>Banani</v>
       </c>
       <c r="C19" t="str">
-        <v>192.168.194.1</v>
+        <v>192.168.19.1</v>
       </c>
       <c r="D19" t="str">
         <v>BDCOM</v>
@@ -950,21 +950,21 @@
         <v>OK</v>
       </c>
       <c r="I19" t="str">
-        <v>sdwan</v>
+        <v>legacy</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B20" t="str">
-        <v>Banani</v>
+        <v>Mirpur</v>
       </c>
       <c r="C20" t="str">
-        <v>192.168.19.1</v>
+        <v>192.168.20.1</v>
       </c>
       <c r="D20" t="str">
-        <v>BDCOM</v>
+        <v>ADN</v>
       </c>
       <c r="E20" t="str">
         <v>DOWN</v>
@@ -979,27 +979,27 @@
         <v>OK</v>
       </c>
       <c r="I20" t="str">
-        <v>legacy</v>
+        <v>sdwan</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B21" t="str">
-        <v>Mymensingh</v>
+        <v>Uttara</v>
       </c>
       <c r="C21" t="str">
-        <v>192.168.32.1</v>
+        <v>192.168.17.1</v>
       </c>
       <c r="D21" t="str">
-        <v>ALAP</v>
+        <v>Bdcom</v>
       </c>
       <c r="E21" t="str">
         <v>DOWN</v>
       </c>
       <c r="F21" t="str">
-        <v>BDCOM</v>
+        <v>Alap</v>
       </c>
       <c r="G21" t="str">
         <v>DOWN</v>
@@ -1008,18 +1008,18 @@
         <v>OK</v>
       </c>
       <c r="I21" t="str">
-        <v>legacy</v>
+        <v>sdwan</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B22" t="str">
-        <v>Mirpur</v>
+        <v>Mouchak</v>
       </c>
       <c r="C22" t="str">
-        <v>192.168.20.1</v>
+        <v>192.168.22.1</v>
       </c>
       <c r="D22" t="str">
         <v>ADN</v>
@@ -1042,22 +1042,22 @@
     </row>
     <row r="23">
       <c r="A23">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B23" t="str">
-        <v>North South Road</v>
+        <v>Mymensingh</v>
       </c>
       <c r="C23" t="str">
-        <v>192.168.13.1</v>
+        <v>192.168.32.1</v>
       </c>
       <c r="D23" t="str">
-        <v>ADN</v>
+        <v>ALAP</v>
       </c>
       <c r="E23" t="str">
         <v>DOWN</v>
       </c>
       <c r="F23" t="str">
-        <v>ALAP</v>
+        <v>BDCOM</v>
       </c>
       <c r="G23" t="str">
         <v>DOWN</v>
@@ -1071,16 +1071,16 @@
     </row>
     <row r="24">
       <c r="A24">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" t="str">
-        <v>Mouchak</v>
+        <v>Zindabazar</v>
       </c>
       <c r="C24" t="str">
-        <v>192.168.22.1</v>
+        <v>192.168.194.1</v>
       </c>
       <c r="D24" t="str">
-        <v>ADN</v>
+        <v>BDCOM</v>
       </c>
       <c r="E24" t="str">
         <v>DOWN</v>
@@ -1100,22 +1100,22 @@
     </row>
     <row r="25">
       <c r="A25">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B25" t="str">
-        <v>Sayedpur</v>
+        <v>Moulvibazar, Sylhet</v>
       </c>
       <c r="C25" t="str">
-        <v>192.168.163.1</v>
+        <v>192.168.196.1</v>
       </c>
       <c r="D25" t="str">
-        <v>BDCOM</v>
+        <v>ALAP</v>
       </c>
       <c r="E25" t="str">
         <v>DOWN</v>
       </c>
       <c r="F25" t="str">
-        <v>AGNI</v>
+        <v>BRACNET</v>
       </c>
       <c r="G25" t="str">
         <v>DOWN</v>
@@ -1129,22 +1129,22 @@
     </row>
     <row r="26">
       <c r="A26">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B26" t="str">
-        <v>Moulvibazar, Sylhet</v>
+        <v>Chowmohoni</v>
       </c>
       <c r="C26" t="str">
-        <v>192.168.196.1</v>
+        <v>192.168.138.1</v>
       </c>
       <c r="D26" t="str">
-        <v>ALAP</v>
+        <v>BDCOM</v>
       </c>
       <c r="E26" t="str">
         <v>DOWN</v>
       </c>
       <c r="F26" t="str">
-        <v>BRACNET</v>
+        <v>ALAP</v>
       </c>
       <c r="G26" t="str">
         <v>DOWN</v>
@@ -1153,18 +1153,18 @@
         <v>OK</v>
       </c>
       <c r="I26" t="str">
-        <v>legacy</v>
+        <v>sdwan</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" t="str">
-        <v>O.R.Nizam</v>
+        <v>Sayedpur</v>
       </c>
       <c r="C27" t="str">
-        <v>192.168.132.1</v>
+        <v>192.168.163.1</v>
       </c>
       <c r="D27" t="str">
         <v>BDCOM</v>
@@ -1173,7 +1173,7 @@
         <v>DOWN</v>
       </c>
       <c r="F27" t="str">
-        <v>ALAP</v>
+        <v>AGNI</v>
       </c>
       <c r="G27" t="str">
         <v>DOWN</v>
@@ -1182,21 +1182,21 @@
         <v>OK</v>
       </c>
       <c r="I27" t="str">
-        <v>sdwan</v>
+        <v>legacy</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B28" t="str">
-        <v>Chowmohoni</v>
+        <v>Dhanmondi</v>
       </c>
       <c r="C28" t="str">
-        <v>192.168.138.1</v>
+        <v>192.168.23.1</v>
       </c>
       <c r="D28" t="str">
-        <v>BDCOM</v>
+        <v>ADN</v>
       </c>
       <c r="E28" t="str">
         <v>DOWN</v>
@@ -1211,18 +1211,18 @@
         <v>OK</v>
       </c>
       <c r="I28" t="str">
-        <v>sdwan</v>
+        <v>legacy</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B29" t="str">
-        <v>Comilla</v>
+        <v>Jessore</v>
       </c>
       <c r="C29" t="str">
-        <v>192.168.134.1</v>
+        <v>192.168.228.1</v>
       </c>
       <c r="D29" t="str">
         <v>ALAP</v>
@@ -1231,7 +1231,7 @@
         <v>DOWN</v>
       </c>
       <c r="F29" t="str">
-        <v>BRACNET</v>
+        <v>AMBER-IT</v>
       </c>
       <c r="G29" t="str">
         <v>DOWN</v>
@@ -1245,13 +1245,13 @@
     </row>
     <row r="30">
       <c r="A30">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" t="str">
-        <v>Jessore</v>
+        <v>Comilla</v>
       </c>
       <c r="C30" t="str">
-        <v>192.168.228.1</v>
+        <v>192.168.134.1</v>
       </c>
       <c r="D30" t="str">
         <v>ALAP</v>
@@ -1260,7 +1260,7 @@
         <v>DOWN</v>
       </c>
       <c r="F30" t="str">
-        <v>AMBER-IT</v>
+        <v>BRACNET</v>
       </c>
       <c r="G30" t="str">
         <v>DOWN</v>
@@ -1274,16 +1274,16 @@
     </row>
     <row r="31">
       <c r="A31">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B31" t="str">
-        <v>Dhanmondi</v>
+        <v>O.R.Nizam</v>
       </c>
       <c r="C31" t="str">
-        <v>192.168.23.1</v>
+        <v>192.168.132.1</v>
       </c>
       <c r="D31" t="str">
-        <v>ADN</v>
+        <v>BDCOM</v>
       </c>
       <c r="E31" t="str">
         <v>DOWN</v>
@@ -1298,7 +1298,7 @@
         <v>OK</v>
       </c>
       <c r="I31" t="str">
-        <v>legacy</v>
+        <v>sdwan</v>
       </c>
     </row>
     <row r="32">
@@ -1361,16 +1361,16 @@
     </row>
     <row r="34">
       <c r="A34">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B34" t="str">
-        <v>Sreemangal</v>
+        <v>Mohammadpur</v>
       </c>
       <c r="C34" t="str">
-        <v>192.168.197.1</v>
+        <v>192.168.24.1</v>
       </c>
       <c r="D34" t="str">
-        <v>BDCOM</v>
+        <v>ADN</v>
       </c>
       <c r="E34" t="str">
         <v>DOWN</v>
@@ -1385,7 +1385,7 @@
         <v>OK</v>
       </c>
       <c r="I34" t="str">
-        <v>legacy</v>
+        <v>sdwan</v>
       </c>
     </row>
     <row r="35">
@@ -1419,16 +1419,16 @@
     </row>
     <row r="36">
       <c r="A36">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B36" t="str">
-        <v>Narayangonj</v>
+        <v>Companigonj</v>
       </c>
       <c r="C36" t="str">
-        <v>192.168.28.1</v>
+        <v>192.168.133.1</v>
       </c>
       <c r="D36" t="str">
-        <v>SQUARE</v>
+        <v>BRACNET</v>
       </c>
       <c r="E36" t="str">
         <v>DOWN</v>
@@ -1448,16 +1448,16 @@
     </row>
     <row r="37">
       <c r="A37">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B37" t="str">
-        <v>Mohammadpur</v>
+        <v>Sreemangal</v>
       </c>
       <c r="C37" t="str">
-        <v>192.168.24.1</v>
+        <v>192.168.197.1</v>
       </c>
       <c r="D37" t="str">
-        <v>ADN</v>
+        <v>BDCOM</v>
       </c>
       <c r="E37" t="str">
         <v>DOWN</v>
@@ -1472,21 +1472,21 @@
         <v>OK</v>
       </c>
       <c r="I37" t="str">
-        <v>sdwan</v>
+        <v>legacy</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38" t="str">
-        <v>Companigonj</v>
+        <v>Narayangonj</v>
       </c>
       <c r="C38" t="str">
-        <v>192.168.133.1</v>
+        <v>192.168.28.1</v>
       </c>
       <c r="D38" t="str">
-        <v>BRACNET</v>
+        <v>SQUARE</v>
       </c>
       <c r="E38" t="str">
         <v>DOWN</v>
@@ -1506,42 +1506,42 @@
     </row>
     <row r="39">
       <c r="A39">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B39" t="str">
-        <v>Joydebpur</v>
+        <v>Beanibazar</v>
       </c>
       <c r="C39" t="str">
-        <v>192.168.31.1</v>
+        <v>192.168.195.1</v>
       </c>
       <c r="D39" t="str">
-        <v/>
+        <v>BDCOM</v>
       </c>
       <c r="E39" t="str">
-        <v>UNKNOWN</v>
+        <v>DOWN</v>
       </c>
       <c r="F39" t="str">
-        <v/>
+        <v>BRACNET</v>
       </c>
       <c r="G39" t="str">
-        <v>UNKNOWN</v>
+        <v>DOWN</v>
       </c>
       <c r="H39" t="str">
-        <v>connect ECONNREFUSED 192.168.31.1:22</v>
+        <v>OK</v>
       </c>
       <c r="I39" t="str">
-        <v>sdwan</v>
+        <v>legacy</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B40" t="str">
-        <v>Kapasia</v>
+        <v>Gallai</v>
       </c>
       <c r="C40" t="str">
-        <v>192.168.30.1</v>
+        <v>192.168.135.1</v>
       </c>
       <c r="D40" t="str">
         <v>ALAP</v>
@@ -1550,7 +1550,7 @@
         <v>DOWN</v>
       </c>
       <c r="F40" t="str">
-        <v>AMBER-IT</v>
+        <v>BDCOM</v>
       </c>
       <c r="G40" t="str">
         <v>DOWN</v>
@@ -1593,22 +1593,22 @@
     </row>
     <row r="42">
       <c r="A42">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B42" t="str">
-        <v>Beanibazar</v>
+        <v>Islampur</v>
       </c>
       <c r="C42" t="str">
-        <v>192.168.195.1</v>
+        <v>192.168.25.1</v>
       </c>
       <c r="D42" t="str">
-        <v>BDCOM</v>
+        <v>ALAP</v>
       </c>
       <c r="E42" t="str">
         <v>DOWN</v>
       </c>
       <c r="F42" t="str">
-        <v>BRACNET</v>
+        <v>KS</v>
       </c>
       <c r="G42" t="str">
         <v>DOWN</v>
@@ -1617,56 +1617,56 @@
         <v>OK</v>
       </c>
       <c r="I42" t="str">
-        <v>legacy</v>
+        <v>sdwan</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43">
-        <v>41</v>
+      <c r="A43" t="str">
+        <v/>
       </c>
       <c r="B43" t="str">
-        <v>Islampur</v>
+        <v/>
       </c>
       <c r="C43" t="str">
-        <v>192.168.25.1</v>
+        <v/>
       </c>
       <c r="D43" t="str">
-        <v>ALAP</v>
+        <v/>
       </c>
       <c r="E43" t="str">
-        <v>DOWN</v>
+        <v>UNKNOWN</v>
       </c>
       <c r="F43" t="str">
-        <v>KS</v>
+        <v/>
       </c>
       <c r="G43" t="str">
-        <v>DOWN</v>
+        <v>UNKNOWN</v>
       </c>
       <c r="H43" t="str">
         <v>OK</v>
       </c>
       <c r="I43" t="str">
-        <v>sdwan</v>
+        <v>UNKNOWN</v>
       </c>
     </row>
     <row r="44">
       <c r="A44">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B44" t="str">
-        <v>Gallai</v>
+        <v>Pragati_sarani</v>
       </c>
       <c r="C44" t="str">
-        <v>192.168.135.1</v>
+        <v>192.168.21.1</v>
       </c>
       <c r="D44" t="str">
-        <v>ALAP</v>
+        <v>ADN</v>
       </c>
       <c r="E44" t="str">
         <v>DOWN</v>
       </c>
       <c r="F44" t="str">
-        <v>BDCOM</v>
+        <v>ALAP</v>
       </c>
       <c r="G44" t="str">
         <v>DOWN</v>
@@ -1709,22 +1709,22 @@
     </row>
     <row r="46">
       <c r="A46">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" t="str">
-        <v>Pragati_sarani</v>
+        <v>Kapasia</v>
       </c>
       <c r="C46" t="str">
-        <v>192.168.21.1</v>
+        <v>192.168.30.1</v>
       </c>
       <c r="D46" t="str">
-        <v>ADN</v>
+        <v>ALAP</v>
       </c>
       <c r="E46" t="str">
         <v>DOWN</v>
       </c>
       <c r="F46" t="str">
-        <v>ALAP</v>
+        <v>AMBER-IT</v>
       </c>
       <c r="G46" t="str">
         <v>DOWN</v>
@@ -1738,22 +1738,22 @@
     </row>
     <row r="47">
       <c r="A47">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B47" t="str">
-        <v>Feni</v>
+        <v>Amborkhana</v>
       </c>
       <c r="C47" t="str">
-        <v>192.168.136.1</v>
+        <v>192.168.198.1</v>
       </c>
       <c r="D47" t="str">
-        <v>BDCOM</v>
+        <v>ALAP</v>
       </c>
       <c r="E47" t="str">
         <v>DOWN</v>
       </c>
       <c r="F47" t="str">
-        <v>ALAP</v>
+        <v>BDCOM</v>
       </c>
       <c r="G47" t="str">
         <v>DOWN</v>
@@ -1762,18 +1762,18 @@
         <v>OK</v>
       </c>
       <c r="I47" t="str">
-        <v>legacy</v>
+        <v>sdwan</v>
       </c>
     </row>
     <row r="48">
       <c r="A48">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B48" t="str">
-        <v>Coxsbazar</v>
+        <v>Hathazari</v>
       </c>
       <c r="C48" t="str">
-        <v>192.168.137.1</v>
+        <v>192.168.139.1</v>
       </c>
       <c r="D48" t="str">
         <v>BDCOM</v>
@@ -1782,7 +1782,7 @@
         <v>DOWN</v>
       </c>
       <c r="F48" t="str">
-        <v>BRACNET</v>
+        <v>ALAP</v>
       </c>
       <c r="G48" t="str">
         <v>DOWN</v>
@@ -1791,18 +1791,18 @@
         <v>OK</v>
       </c>
       <c r="I48" t="str">
-        <v>mikrotik</v>
+        <v>sdwan</v>
       </c>
     </row>
     <row r="49">
       <c r="A49">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" t="str">
-        <v>Hathazari</v>
+        <v>Coxsbazar</v>
       </c>
       <c r="C49" t="str">
-        <v>192.168.139.1</v>
+        <v>192.168.137.1</v>
       </c>
       <c r="D49" t="str">
         <v>BDCOM</v>
@@ -1811,7 +1811,7 @@
         <v>DOWN</v>
       </c>
       <c r="F49" t="str">
-        <v>ALAP</v>
+        <v>BRACNET</v>
       </c>
       <c r="G49" t="str">
         <v>DOWN</v>
@@ -1820,27 +1820,27 @@
         <v>OK</v>
       </c>
       <c r="I49" t="str">
-        <v>sdwan</v>
+        <v>mikrotik</v>
       </c>
     </row>
     <row r="50">
       <c r="A50">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B50" t="str">
-        <v>Amborkhana</v>
+        <v>Bhairab</v>
       </c>
       <c r="C50" t="str">
-        <v>192.168.198.1</v>
+        <v>192.168.35.1</v>
       </c>
       <c r="D50" t="str">
-        <v>ALAP</v>
+        <v>BRACNET</v>
       </c>
       <c r="E50" t="str">
         <v>DOWN</v>
       </c>
       <c r="F50" t="str">
-        <v>BDCOM</v>
+        <v>ALAP</v>
       </c>
       <c r="G50" t="str">
         <v>DOWN</v>
@@ -1849,7 +1849,7 @@
         <v>OK</v>
       </c>
       <c r="I50" t="str">
-        <v>sdwan</v>
+        <v>legacy</v>
       </c>
     </row>
     <row r="51">
@@ -1883,22 +1883,22 @@
     </row>
     <row r="52">
       <c r="A52">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B52" t="str">
-        <v>Gulshan</v>
+        <v>Feni</v>
       </c>
       <c r="C52" t="str">
-        <v>192.168.36.1</v>
+        <v>192.168.136.1</v>
       </c>
       <c r="D52" t="str">
-        <v>BRACNET</v>
+        <v>BDCOM</v>
       </c>
       <c r="E52" t="str">
         <v>DOWN</v>
       </c>
       <c r="F52" t="str">
-        <v>SQUARE</v>
+        <v>ALAP</v>
       </c>
       <c r="G52" t="str">
         <v>DOWN</v>
@@ -1912,22 +1912,22 @@
     </row>
     <row r="53">
       <c r="A53">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B53" t="str">
-        <v>Jatrabari</v>
+        <v>Jhalokathi</v>
       </c>
       <c r="C53" t="str">
-        <v>192.168.34.1</v>
+        <v>192.168.242.1</v>
       </c>
       <c r="D53" t="str">
-        <v>KS</v>
+        <v>BRACNET</v>
       </c>
       <c r="E53" t="str">
         <v>DOWN</v>
       </c>
       <c r="F53" t="str">
-        <v>ALAP</v>
+        <v>BDCOM</v>
       </c>
       <c r="G53" t="str">
         <v>DOWN</v>
@@ -1936,27 +1936,27 @@
         <v>OK</v>
       </c>
       <c r="I53" t="str">
-        <v>sdwan</v>
+        <v>legacy</v>
       </c>
     </row>
     <row r="54">
       <c r="A54">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B54" t="str">
-        <v>Bhairab</v>
+        <v>Chuknagar</v>
       </c>
       <c r="C54" t="str">
-        <v>192.168.35.1</v>
+        <v>192.168.230.1</v>
       </c>
       <c r="D54" t="str">
-        <v>BRACNET</v>
+        <v>AMBER-IT</v>
       </c>
       <c r="E54" t="str">
         <v>DOWN</v>
       </c>
       <c r="F54" t="str">
-        <v>ALAP</v>
+        <v>A.D.N</v>
       </c>
       <c r="G54" t="str">
         <v>DOWN</v>
@@ -1970,13 +1970,13 @@
     </row>
     <row r="55">
       <c r="A55">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B55" t="str">
-        <v>Jhalokathi</v>
+        <v>Hazaribagh</v>
       </c>
       <c r="C55" t="str">
-        <v>192.168.242.1</v>
+        <v>192.168.38.1</v>
       </c>
       <c r="D55" t="str">
         <v>BRACNET</v>
@@ -1985,7 +1985,7 @@
         <v>DOWN</v>
       </c>
       <c r="F55" t="str">
-        <v>BDCOM</v>
+        <v>KS</v>
       </c>
       <c r="G55" t="str">
         <v>DOWN</v>
@@ -1999,22 +1999,22 @@
     </row>
     <row r="56">
       <c r="A56">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B56" t="str">
-        <v>Chuknagar</v>
+        <v>Gulshan</v>
       </c>
       <c r="C56" t="str">
-        <v>192.168.230.1</v>
+        <v>192.168.36.1</v>
       </c>
       <c r="D56" t="str">
-        <v>AMBER-IT</v>
+        <v>BRACNET</v>
       </c>
       <c r="E56" t="str">
         <v>DOWN</v>
       </c>
       <c r="F56" t="str">
-        <v>A.D.N</v>
+        <v>SQUARE</v>
       </c>
       <c r="G56" t="str">
         <v>DOWN</v>
@@ -2028,22 +2028,22 @@
     </row>
     <row r="57">
       <c r="A57">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B57" t="str">
-        <v>Mongla</v>
+        <v>Jatrabari</v>
       </c>
       <c r="C57" t="str">
-        <v>192.168.229.1</v>
+        <v>192.168.34.1</v>
       </c>
       <c r="D57" t="str">
-        <v>BRACNET</v>
+        <v>KS</v>
       </c>
       <c r="E57" t="str">
         <v>DOWN</v>
       </c>
       <c r="F57" t="str">
-        <v>SQUARE</v>
+        <v>ALAP</v>
       </c>
       <c r="G57" t="str">
         <v>DOWN</v>
@@ -2052,27 +2052,27 @@
         <v>OK</v>
       </c>
       <c r="I57" t="str">
-        <v>legacy</v>
+        <v>sdwan</v>
       </c>
     </row>
     <row r="58">
       <c r="A58">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B58" t="str">
-        <v>Keranigonj</v>
+        <v>Manda</v>
       </c>
       <c r="C58" t="str">
-        <v>192.168.37.1</v>
+        <v>192.168.39.1</v>
       </c>
       <c r="D58" t="str">
-        <v>BRACNET</v>
+        <v>ALAP</v>
       </c>
       <c r="E58" t="str">
         <v>DOWN</v>
       </c>
       <c r="F58" t="str">
-        <v>AMBER-IT</v>
+        <v>KS</v>
       </c>
       <c r="G58" t="str">
         <v>DOWN</v>
@@ -2081,7 +2081,7 @@
         <v>OK</v>
       </c>
       <c r="I58" t="str">
-        <v>legacy</v>
+        <v>sdwan</v>
       </c>
     </row>
     <row r="59">
@@ -2115,13 +2115,13 @@
     </row>
     <row r="60">
       <c r="A60">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B60" t="str">
-        <v>Hazaribagh</v>
+        <v>Mongla</v>
       </c>
       <c r="C60" t="str">
-        <v>192.168.38.1</v>
+        <v>192.168.229.1</v>
       </c>
       <c r="D60" t="str">
         <v>BRACNET</v>
@@ -2130,7 +2130,7 @@
         <v>DOWN</v>
       </c>
       <c r="F60" t="str">
-        <v>KS</v>
+        <v>SQUARE</v>
       </c>
       <c r="G60" t="str">
         <v>DOWN</v>
@@ -2144,22 +2144,22 @@
     </row>
     <row r="61">
       <c r="A61">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B61" t="str">
-        <v>Manda</v>
+        <v>Keranigonj</v>
       </c>
       <c r="C61" t="str">
-        <v>192.168.39.1</v>
+        <v>192.168.37.1</v>
       </c>
       <c r="D61" t="str">
-        <v>ALAP</v>
+        <v>BRACNET</v>
       </c>
       <c r="E61" t="str">
         <v>DOWN</v>
       </c>
       <c r="F61" t="str">
-        <v>KS</v>
+        <v>AMBER-IT</v>
       </c>
       <c r="G61" t="str">
         <v>DOWN</v>
@@ -2168,7 +2168,7 @@
         <v>OK</v>
       </c>
       <c r="I61" t="str">
-        <v>sdwan</v>
+        <v>legacy</v>
       </c>
     </row>
     <row r="62">
@@ -2202,13 +2202,13 @@
     </row>
     <row r="63">
       <c r="A63">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B63" t="str">
-        <v>Mothbaria</v>
+        <v>Tontor bazar</v>
       </c>
       <c r="C63" t="str">
-        <v>192.168.243.1</v>
+        <v>192.168.142.1</v>
       </c>
       <c r="D63" t="str">
         <v>BDCOM</v>
@@ -2217,7 +2217,7 @@
         <v>DOWN</v>
       </c>
       <c r="F63" t="str">
-        <v>LINK3</v>
+        <v>AMBER-IT</v>
       </c>
       <c r="G63" t="str">
         <v>DOWN</v>
@@ -2231,13 +2231,13 @@
     </row>
     <row r="64">
       <c r="A64">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B64" t="str">
-        <v>B.Baria</v>
+        <v>Mothbaria</v>
       </c>
       <c r="C64" t="str">
-        <v>192.168.141.1</v>
+        <v>192.168.243.1</v>
       </c>
       <c r="D64" t="str">
         <v>BDCOM</v>
@@ -2246,7 +2246,7 @@
         <v>DOWN</v>
       </c>
       <c r="F64" t="str">
-        <v>SQUARE</v>
+        <v>LINK3</v>
       </c>
       <c r="G64" t="str">
         <v>DOWN</v>
@@ -2260,22 +2260,22 @@
     </row>
     <row r="65">
       <c r="A65">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B65" t="str">
-        <v>Tontor bazar</v>
+        <v>Hemayatpur</v>
       </c>
       <c r="C65" t="str">
-        <v>192.168.142.1</v>
+        <v>192.168.41.1</v>
       </c>
       <c r="D65" t="str">
-        <v>BDCOM</v>
+        <v>ALAP</v>
       </c>
       <c r="E65" t="str">
         <v>DOWN</v>
       </c>
       <c r="F65" t="str">
-        <v>AMBER-IT</v>
+        <v>BDCOM</v>
       </c>
       <c r="G65" t="str">
         <v>DOWN</v>
@@ -2289,13 +2289,13 @@
     </row>
     <row r="66">
       <c r="A66">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B66" t="str">
-        <v>Bodorgonj</v>
+        <v>B.Baria</v>
       </c>
       <c r="C66" t="str">
-        <v>192.168.165.1</v>
+        <v>192.168.141.1</v>
       </c>
       <c r="D66" t="str">
         <v>BDCOM</v>
@@ -2304,7 +2304,7 @@
         <v>DOWN</v>
       </c>
       <c r="F66" t="str">
-        <v>BRACNET</v>
+        <v>SQUARE</v>
       </c>
       <c r="G66" t="str">
         <v>DOWN</v>
@@ -2318,22 +2318,22 @@
     </row>
     <row r="67">
       <c r="A67">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B67" t="str">
-        <v>Abdullahpur</v>
+        <v>Bodorgonj</v>
       </c>
       <c r="C67" t="str">
-        <v>192.168.43.1</v>
+        <v>192.168.165.1</v>
       </c>
       <c r="D67" t="str">
-        <v>IOL</v>
+        <v>BDCOM</v>
       </c>
       <c r="E67" t="str">
         <v>DOWN</v>
       </c>
       <c r="F67" t="str">
-        <v>BDCOM</v>
+        <v>BRACNET</v>
       </c>
       <c r="G67" t="str">
         <v>DOWN</v>
@@ -2347,16 +2347,16 @@
     </row>
     <row r="68">
       <c r="A68">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B68" t="str">
-        <v>Bondor</v>
+        <v>Abdullahpur</v>
       </c>
       <c r="C68" t="str">
-        <v>192.168.44.1</v>
+        <v>192.168.43.1</v>
       </c>
       <c r="D68" t="str">
-        <v>PCL</v>
+        <v>IOL</v>
       </c>
       <c r="E68" t="str">
         <v>DOWN</v>
@@ -2376,22 +2376,22 @@
     </row>
     <row r="69">
       <c r="A69">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B69" t="str">
-        <v>Akhaura</v>
+        <v>Bhola</v>
       </c>
       <c r="C69" t="str">
-        <v>192.168.143.1</v>
+        <v>192.168.244.1</v>
       </c>
       <c r="D69" t="str">
-        <v>BDCOM</v>
+        <v>LINK3</v>
       </c>
       <c r="E69" t="str">
         <v>DOWN</v>
       </c>
       <c r="F69" t="str">
-        <v>LINK3</v>
+        <v>A.D.N</v>
       </c>
       <c r="G69" t="str">
         <v>DOWN</v>
@@ -2405,16 +2405,16 @@
     </row>
     <row r="70">
       <c r="A70">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B70" t="str">
-        <v>Hemayatpur</v>
+        <v>Kamrangirchar</v>
       </c>
       <c r="C70" t="str">
-        <v>192.168.41.1</v>
+        <v>192.168.42.1</v>
       </c>
       <c r="D70" t="str">
-        <v>ALAP</v>
+        <v>KS</v>
       </c>
       <c r="E70" t="str">
         <v>DOWN</v>
@@ -2434,22 +2434,22 @@
     </row>
     <row r="71">
       <c r="A71">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B71" t="str">
-        <v>Kamrangirchar</v>
+        <v>Akhaura</v>
       </c>
       <c r="C71" t="str">
-        <v>192.168.42.1</v>
+        <v>192.168.143.1</v>
       </c>
       <c r="D71" t="str">
-        <v>KS</v>
+        <v>BDCOM</v>
       </c>
       <c r="E71" t="str">
         <v>DOWN</v>
       </c>
       <c r="F71" t="str">
-        <v>BDCOM</v>
+        <v>LINK3</v>
       </c>
       <c r="G71" t="str">
         <v>DOWN</v>
@@ -2463,22 +2463,22 @@
     </row>
     <row r="72">
       <c r="A72">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B72" t="str">
-        <v>Madhabpur</v>
+        <v>Khilkhet</v>
       </c>
       <c r="C72" t="str">
-        <v>192.168.199.1</v>
+        <v>192.168.45.1</v>
       </c>
       <c r="D72" t="str">
-        <v>BDCOM</v>
+        <v>ALAP</v>
       </c>
       <c r="E72" t="str">
         <v>DOWN</v>
       </c>
       <c r="F72" t="str">
-        <v>BRACNET</v>
+        <v>BDCOM</v>
       </c>
       <c r="G72" t="str">
         <v>DOWN</v>
@@ -2487,27 +2487,27 @@
         <v>OK</v>
       </c>
       <c r="I72" t="str">
-        <v>legacy</v>
+        <v>sdwan</v>
       </c>
     </row>
     <row r="73">
       <c r="A73">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B73" t="str">
-        <v>Bhola</v>
+        <v>Bondor</v>
       </c>
       <c r="C73" t="str">
-        <v>192.168.244.1</v>
+        <v>192.168.44.1</v>
       </c>
       <c r="D73" t="str">
-        <v>LINK3</v>
+        <v>PCL</v>
       </c>
       <c r="E73" t="str">
         <v>DOWN</v>
       </c>
       <c r="F73" t="str">
-        <v>A.D.N</v>
+        <v>BDCOM</v>
       </c>
       <c r="G73" t="str">
         <v>DOWN</v>
@@ -2521,22 +2521,22 @@
     </row>
     <row r="74">
       <c r="A74">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B74" t="str">
-        <v>Khilkhet</v>
+        <v>Madhabpur</v>
       </c>
       <c r="C74" t="str">
-        <v>192.168.45.1</v>
+        <v>192.168.199.1</v>
       </c>
       <c r="D74" t="str">
-        <v>ALAP</v>
+        <v>BDCOM</v>
       </c>
       <c r="E74" t="str">
         <v>DOWN</v>
       </c>
       <c r="F74" t="str">
-        <v>BDCOM</v>
+        <v>BRACNET</v>
       </c>
       <c r="G74" t="str">
         <v>DOWN</v>
@@ -2545,18 +2545,18 @@
         <v>OK</v>
       </c>
       <c r="I74" t="str">
-        <v>sdwan</v>
+        <v>legacy</v>
       </c>
     </row>
     <row r="75">
       <c r="A75">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B75" t="str">
-        <v>Dinajpur</v>
+        <v>Mirpur-10</v>
       </c>
       <c r="C75" t="str">
-        <v>192.168.166.1</v>
+        <v>192.168.46.1</v>
       </c>
       <c r="D75" t="str">
         <v>BDCOM</v>
@@ -2574,18 +2574,18 @@
         <v>OK</v>
       </c>
       <c r="I75" t="str">
-        <v>legacy</v>
+        <v>sdwan</v>
       </c>
     </row>
     <row r="76">
       <c r="A76">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B76" t="str">
-        <v>Mirpur-10</v>
+        <v>Dinajpur</v>
       </c>
       <c r="C76" t="str">
-        <v>192.168.46.1</v>
+        <v>192.168.166.1</v>
       </c>
       <c r="D76" t="str">
         <v>BDCOM</v>
@@ -2603,18 +2603,18 @@
         <v>OK</v>
       </c>
       <c r="I76" t="str">
-        <v>sdwan</v>
+        <v>legacy</v>
       </c>
     </row>
     <row r="77">
       <c r="A77">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B77" t="str">
-        <v>South Jatrabari</v>
+        <v>Gazipur</v>
       </c>
       <c r="C77" t="str">
-        <v>192.168.48.1</v>
+        <v>192.168.47.1</v>
       </c>
       <c r="D77" t="str">
         <v>BDCOM</v>
@@ -2632,18 +2632,18 @@
         <v>OK</v>
       </c>
       <c r="I77" t="str">
-        <v>sdwan</v>
+        <v>legacy</v>
       </c>
     </row>
     <row r="78">
       <c r="A78">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B78" t="str">
-        <v>Gazipur</v>
+        <v>South Jatrabari</v>
       </c>
       <c r="C78" t="str">
-        <v>192.168.47.1</v>
+        <v>192.168.48.1</v>
       </c>
       <c r="D78" t="str">
         <v>BDCOM</v>
@@ -2661,27 +2661,27 @@
         <v>OK</v>
       </c>
       <c r="I78" t="str">
-        <v>legacy</v>
+        <v>sdwan</v>
       </c>
     </row>
     <row r="79">
       <c r="A79">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B79" t="str">
-        <v>Panchdona</v>
+        <v>Bashurhat</v>
       </c>
       <c r="C79" t="str">
-        <v>192.168.49.1</v>
+        <v>192.168.144.1</v>
       </c>
       <c r="D79" t="str">
-        <v>AMBER-IT</v>
+        <v>BDCOM</v>
       </c>
       <c r="E79" t="str">
         <v>DOWN</v>
       </c>
       <c r="F79" t="str">
-        <v>ALAP</v>
+        <v>BRACNET</v>
       </c>
       <c r="G79" t="str">
         <v>DOWN</v>
@@ -2695,22 +2695,22 @@
     </row>
     <row r="80">
       <c r="A80">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B80" t="str">
-        <v>Bashurhat</v>
+        <v>Kolatia</v>
       </c>
       <c r="C80" t="str">
-        <v>192.168.144.1</v>
+        <v>192.168.50.1</v>
       </c>
       <c r="D80" t="str">
-        <v>BDCOM</v>
+        <v>BRACNET</v>
       </c>
       <c r="E80" t="str">
         <v>DOWN</v>
       </c>
       <c r="F80" t="str">
-        <v>BRACNET</v>
+        <v>BDCOM</v>
       </c>
       <c r="G80" t="str">
         <v>DOWN</v>
@@ -2719,27 +2719,27 @@
         <v>OK</v>
       </c>
       <c r="I80" t="str">
-        <v>legacy</v>
+        <v>sdwan</v>
       </c>
     </row>
     <row r="81">
       <c r="A81">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B81" t="str">
-        <v>Shahzadpur</v>
+        <v>Panchdona</v>
       </c>
       <c r="C81" t="str">
-        <v>192.168.167.1</v>
+        <v>192.168.49.1</v>
       </c>
       <c r="D81" t="str">
-        <v>BRACNET</v>
+        <v>AMBER-IT</v>
       </c>
       <c r="E81" t="str">
         <v>DOWN</v>
       </c>
       <c r="F81" t="str">
-        <v>AMBER-IT</v>
+        <v>ALAP</v>
       </c>
       <c r="G81" t="str">
         <v>DOWN</v>
@@ -2753,13 +2753,13 @@
     </row>
     <row r="82">
       <c r="A82">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B82" t="str">
-        <v>Natunbazar</v>
+        <v>Shahzadpur</v>
       </c>
       <c r="C82" t="str">
-        <v>192.168.54.1</v>
+        <v>192.168.167.1</v>
       </c>
       <c r="D82" t="str">
         <v>BRACNET</v>
@@ -2768,7 +2768,7 @@
         <v>DOWN</v>
       </c>
       <c r="F82" t="str">
-        <v>BDCOM</v>
+        <v>AMBER-IT</v>
       </c>
       <c r="G82" t="str">
         <v>DOWN</v>
@@ -2782,13 +2782,13 @@
     </row>
     <row r="83">
       <c r="A83">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B83" t="str">
-        <v>Kolatia</v>
+        <v>Hajigonj</v>
       </c>
       <c r="C83" t="str">
-        <v>192.168.50.1</v>
+        <v>192.168.145.1</v>
       </c>
       <c r="D83" t="str">
         <v>BRACNET</v>
@@ -2797,7 +2797,7 @@
         <v>DOWN</v>
       </c>
       <c r="F83" t="str">
-        <v>BDCOM</v>
+        <v>AMBER-IT</v>
       </c>
       <c r="G83" t="str">
         <v>DOWN</v>
@@ -2806,18 +2806,18 @@
         <v>OK</v>
       </c>
       <c r="I83" t="str">
-        <v>sdwan</v>
+        <v>legacy</v>
       </c>
     </row>
     <row r="84">
       <c r="A84">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B84" t="str">
-        <v>Hajigonj</v>
+        <v>Panthopath</v>
       </c>
       <c r="C84" t="str">
-        <v>192.168.145.1</v>
+        <v>192.168.52.1</v>
       </c>
       <c r="D84" t="str">
         <v>BRACNET</v>
@@ -2826,7 +2826,7 @@
         <v>DOWN</v>
       </c>
       <c r="F84" t="str">
-        <v>AMBER-IT</v>
+        <v>SQUARE</v>
       </c>
       <c r="G84" t="str">
         <v>DOWN</v>
@@ -2835,27 +2835,27 @@
         <v>OK</v>
       </c>
       <c r="I84" t="str">
-        <v>legacy</v>
+        <v>sdwan</v>
       </c>
     </row>
     <row r="85">
       <c r="A85">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B85" t="str">
-        <v>Panthopath</v>
+        <v>Kutibazar</v>
       </c>
       <c r="C85" t="str">
-        <v>192.168.52.1</v>
+        <v>192.168.147.1</v>
       </c>
       <c r="D85" t="str">
-        <v>BRACNET</v>
+        <v>BDCOM</v>
       </c>
       <c r="E85" t="str">
         <v>DOWN</v>
       </c>
       <c r="F85" t="str">
-        <v>SQUARE</v>
+        <v>AMBER-IT</v>
       </c>
       <c r="G85" t="str">
         <v>DOWN</v>
@@ -2864,27 +2864,27 @@
         <v>OK</v>
       </c>
       <c r="I85" t="str">
-        <v>sdwan</v>
+        <v>legacy</v>
       </c>
     </row>
     <row r="86">
       <c r="A86">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B86" t="str">
-        <v>Kutibazar</v>
+        <v>Natunbazar</v>
       </c>
       <c r="C86" t="str">
-        <v>192.168.147.1</v>
+        <v>192.168.54.1</v>
       </c>
       <c r="D86" t="str">
-        <v>BDCOM</v>
+        <v>BRACNET</v>
       </c>
       <c r="E86" t="str">
         <v>DOWN</v>
       </c>
       <c r="F86" t="str">
-        <v>AMBER-IT</v>
+        <v>BDCOM</v>
       </c>
       <c r="G86" t="str">
         <v>DOWN</v>
@@ -2927,71 +2927,71 @@
     </row>
     <row r="88">
       <c r="A88">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B88" t="str">
-        <v>Dokkhinkhan</v>
+        <v>Stationroad</v>
       </c>
       <c r="C88" t="str">
-        <v>192.168.53.1</v>
+        <v>192.168.146.1</v>
       </c>
       <c r="D88" t="str">
+        <v>BRACNET</v>
+      </c>
+      <c r="E88" t="str">
+        <v>DOWN</v>
+      </c>
+      <c r="F88" t="str">
+        <v>ALAP</v>
+      </c>
+      <c r="G88" t="str">
+        <v>DOWN</v>
+      </c>
+      <c r="H88" t="str">
+        <v>OK</v>
+      </c>
+      <c r="I88" t="str">
+        <v>legacy</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
         <v/>
       </c>
-      <c r="E88" t="str">
+      <c r="B89" t="str">
+        <v/>
+      </c>
+      <c r="C89" t="str">
+        <v/>
+      </c>
+      <c r="D89" t="str">
+        <v/>
+      </c>
+      <c r="E89" t="str">
         <v>UNKNOWN</v>
       </c>
-      <c r="F88" t="str">
+      <c r="F89" t="str">
         <v/>
       </c>
-      <c r="G88" t="str">
+      <c r="G89" t="str">
         <v>UNKNOWN</v>
       </c>
-      <c r="H88" t="str">
-        <v>connect ECONNREFUSED 192.168.53.1:22</v>
-      </c>
-      <c r="I88" t="str">
-        <v>legacy</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89">
-        <v>90</v>
-      </c>
-      <c r="B89" t="str">
-        <v>Rahimanogor</v>
-      </c>
-      <c r="C89" t="str">
-        <v>192.168.148.1</v>
-      </c>
-      <c r="D89" t="str">
-        <v>ALAP</v>
-      </c>
-      <c r="E89" t="str">
-        <v>DOWN</v>
-      </c>
-      <c r="F89" t="str">
-        <v>LINK3</v>
-      </c>
-      <c r="G89" t="str">
-        <v>DOWN</v>
-      </c>
       <c r="H89" t="str">
         <v>OK</v>
       </c>
       <c r="I89" t="str">
-        <v>legacy</v>
+        <v>UNKNOWN</v>
       </c>
     </row>
     <row r="90">
       <c r="A90">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B90" t="str">
-        <v>Stationroad</v>
+        <v>Shymoli</v>
       </c>
       <c r="C90" t="str">
-        <v>192.168.146.1</v>
+        <v>192.168.55.1</v>
       </c>
       <c r="D90" t="str">
         <v>BRACNET</v>
@@ -3000,7 +3000,7 @@
         <v>DOWN</v>
       </c>
       <c r="F90" t="str">
-        <v>ALAP</v>
+        <v>BDCOM</v>
       </c>
       <c r="G90" t="str">
         <v>DOWN</v>
@@ -3009,27 +3009,27 @@
         <v>OK</v>
       </c>
       <c r="I90" t="str">
-        <v>legacy</v>
+        <v>sdwan</v>
       </c>
     </row>
     <row r="91">
       <c r="A91">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B91" t="str">
-        <v>Shymoli</v>
+        <v>Rahimanogor</v>
       </c>
       <c r="C91" t="str">
-        <v>192.168.55.1</v>
+        <v>192.168.148.1</v>
       </c>
       <c r="D91" t="str">
-        <v>BRACNET</v>
+        <v>ALAP</v>
       </c>
       <c r="E91" t="str">
         <v>DOWN</v>
       </c>
       <c r="F91" t="str">
-        <v>BDCOM</v>
+        <v>LINK3</v>
       </c>
       <c r="G91" t="str">
         <v>DOWN</v>
@@ -3038,18 +3038,18 @@
         <v>OK</v>
       </c>
       <c r="I91" t="str">
-        <v>sdwan</v>
+        <v>legacy</v>
       </c>
     </row>
     <row r="92">
       <c r="A92">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B92" t="str">
-        <v>Valanagar</v>
+        <v>Kathgora</v>
       </c>
       <c r="C92" t="str">
-        <v>192.168.56.1</v>
+        <v>192.168.57.1</v>
       </c>
       <c r="D92" t="str">
         <v>ALAP</v>
@@ -3058,7 +3058,7 @@
         <v>DOWN</v>
       </c>
       <c r="F92" t="str">
-        <v>AMBER-IT</v>
+        <v>BDCOM</v>
       </c>
       <c r="G92" t="str">
         <v>DOWN</v>
@@ -3067,18 +3067,18 @@
         <v>OK</v>
       </c>
       <c r="I92" t="str">
-        <v>legacy</v>
+        <v>sdwan</v>
       </c>
     </row>
     <row r="93">
       <c r="A93">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B93" t="str">
-        <v>Kathgora</v>
+        <v>Valanagar</v>
       </c>
       <c r="C93" t="str">
-        <v>192.168.57.1</v>
+        <v>192.168.56.1</v>
       </c>
       <c r="D93" t="str">
         <v>ALAP</v>
@@ -3087,7 +3087,7 @@
         <v>DOWN</v>
       </c>
       <c r="F93" t="str">
-        <v>BDCOM</v>
+        <v>AMBER-IT</v>
       </c>
       <c r="G93" t="str">
         <v>DOWN</v>
@@ -3096,21 +3096,21 @@
         <v>OK</v>
       </c>
       <c r="I93" t="str">
-        <v>sdwan</v>
+        <v>legacy</v>
       </c>
     </row>
     <row r="94">
       <c r="A94">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B94" t="str">
-        <v>Pabna</v>
+        <v>Ruhitpur</v>
       </c>
       <c r="C94" t="str">
-        <v>192.168.168.1</v>
+        <v>192.168.59.1</v>
       </c>
       <c r="D94" t="str">
-        <v>BDCOM</v>
+        <v>KS</v>
       </c>
       <c r="E94" t="str">
         <v>DOWN</v>
@@ -3130,16 +3130,16 @@
     </row>
     <row r="95">
       <c r="A95">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B95" t="str">
-        <v>Ruhitpur</v>
+        <v>Halishohor</v>
       </c>
       <c r="C95" t="str">
-        <v>192.168.59.1</v>
+        <v>192.168.149.1</v>
       </c>
       <c r="D95" t="str">
-        <v>KS</v>
+        <v>BDCOM</v>
       </c>
       <c r="E95" t="str">
         <v>DOWN</v>
@@ -3159,13 +3159,13 @@
     </row>
     <row r="96">
       <c r="A96">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B96" t="str">
-        <v>Halishohor</v>
+        <v>Pabna</v>
       </c>
       <c r="C96" t="str">
-        <v>192.168.149.1</v>
+        <v>192.168.168.1</v>
       </c>
       <c r="D96" t="str">
         <v>BDCOM</v>
@@ -3188,16 +3188,16 @@
     </row>
     <row r="97">
       <c r="A97">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B97" t="str">
-        <v>Rangpur</v>
+        <v>Noyapur</v>
       </c>
       <c r="C97" t="str">
-        <v>192.168.169.1</v>
+        <v>192.168.60.1</v>
       </c>
       <c r="D97" t="str">
-        <v>BDCOM</v>
+        <v>BRACNET</v>
       </c>
       <c r="E97" t="str">
         <v>DOWN</v>
@@ -3217,22 +3217,22 @@
     </row>
     <row r="98">
       <c r="A98">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B98" t="str">
-        <v>Gollamari</v>
+        <v>Uttara Janapath</v>
       </c>
       <c r="C98" t="str">
-        <v>192.168.231.1</v>
+        <v>192.168.58.1</v>
       </c>
       <c r="D98" t="str">
-        <v>BDCOM</v>
+        <v>ALAP</v>
       </c>
       <c r="E98" t="str">
         <v>DOWN</v>
       </c>
       <c r="F98" t="str">
-        <v>ALAP</v>
+        <v>BDCOM</v>
       </c>
       <c r="G98" t="str">
         <v>DOWN</v>
@@ -3241,18 +3241,18 @@
         <v>OK</v>
       </c>
       <c r="I98" t="str">
-        <v>legacy</v>
+        <v>sdwan</v>
       </c>
     </row>
     <row r="99">
       <c r="A99">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B99" t="str">
-        <v>Uttara Janapath</v>
+        <v>Bormi</v>
       </c>
       <c r="C99" t="str">
-        <v>192.168.58.1</v>
+        <v>192.168.62.1</v>
       </c>
       <c r="D99" t="str">
         <v>ALAP</v>
@@ -3270,18 +3270,18 @@
         <v>OK</v>
       </c>
       <c r="I99" t="str">
-        <v>sdwan</v>
+        <v>legacy</v>
       </c>
     </row>
     <row r="100">
       <c r="A100">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B100" t="str">
-        <v>Rampura</v>
+        <v>Rangpur</v>
       </c>
       <c r="C100" t="str">
-        <v>192.168.63.1</v>
+        <v>192.168.169.1</v>
       </c>
       <c r="D100" t="str">
         <v>BDCOM</v>
@@ -3299,27 +3299,27 @@
         <v>OK</v>
       </c>
       <c r="I100" t="str">
-        <v>sdwan</v>
+        <v>legacy</v>
       </c>
     </row>
     <row r="101">
       <c r="A101">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B101" t="str">
-        <v>Bormi</v>
+        <v>Gollamari</v>
       </c>
       <c r="C101" t="str">
-        <v>192.168.62.1</v>
+        <v>192.168.231.1</v>
       </c>
       <c r="D101" t="str">
-        <v>ALAP</v>
+        <v>BDCOM</v>
       </c>
       <c r="E101" t="str">
         <v>DOWN</v>
       </c>
       <c r="F101" t="str">
-        <v>BDCOM</v>
+        <v>ALAP</v>
       </c>
       <c r="G101" t="str">
         <v>DOWN</v>
@@ -3333,22 +3333,22 @@
     </row>
     <row r="102">
       <c r="A102">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B102" t="str">
-        <v>Teknaf</v>
+        <v>Rampal</v>
       </c>
       <c r="C102" t="str">
-        <v>192.168.150.1</v>
+        <v>192.168.61.1</v>
       </c>
       <c r="D102" t="str">
-        <v>AMBER-IT</v>
+        <v>BRACNET</v>
       </c>
       <c r="E102" t="str">
         <v>DOWN</v>
       </c>
       <c r="F102" t="str">
-        <v>BRACNET</v>
+        <v>ALAP</v>
       </c>
       <c r="G102" t="str">
         <v>DOWN</v>
@@ -3357,7 +3357,7 @@
         <v>OK</v>
       </c>
       <c r="I102" t="str">
-        <v>legacy</v>
+        <v>sdwan</v>
       </c>
     </row>
     <row r="103">
@@ -3391,22 +3391,22 @@
     </row>
     <row r="104">
       <c r="A104">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B104" t="str">
-        <v>Noyapur</v>
+        <v>Teknaf</v>
       </c>
       <c r="C104" t="str">
-        <v>192.168.60.1</v>
+        <v>192.168.150.1</v>
       </c>
       <c r="D104" t="str">
+        <v>AMBER-IT</v>
+      </c>
+      <c r="E104" t="str">
+        <v>DOWN</v>
+      </c>
+      <c r="F104" t="str">
         <v>BRACNET</v>
-      </c>
-      <c r="E104" t="str">
-        <v>DOWN</v>
-      </c>
-      <c r="F104" t="str">
-        <v>ALAP</v>
       </c>
       <c r="G104" t="str">
         <v>DOWN</v>
@@ -3420,16 +3420,16 @@
     </row>
     <row r="105">
       <c r="A105">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B105" t="str">
-        <v>Rampal</v>
+        <v>Rampura</v>
       </c>
       <c r="C105" t="str">
-        <v>192.168.61.1</v>
+        <v>192.168.63.1</v>
       </c>
       <c r="D105" t="str">
-        <v>BRACNET</v>
+        <v>BDCOM</v>
       </c>
       <c r="E105" t="str">
         <v>DOWN</v>

</xml_diff>